<commit_message>
support alpha&beta and batch-gemm
</commit_message>
<xml_diff>
--- a/doc/480x512 kernel analysis.xlsx
+++ b/doc/480x512 kernel analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\srdccmode-corp\home1\feiw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\TensileLite\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B06F385-6CB4-47C9-A080-3707ED012FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3ED150-09AB-488D-BF39-972328B0ACB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12645" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -649,100 +649,100 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -853,6 +853,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-95B9-4523-9A25-B4B5DE506AD1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -868,6 +873,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-95B9-4523-9A25-B4B5DE506AD1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -883,6 +893,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-95B9-4523-9A25-B4B5DE506AD1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -898,6 +913,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-95B9-4523-9A25-B4B5DE506AD1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -913,6 +933,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-95B9-4523-9A25-B4B5DE506AD1}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -1762,6 +1787,56 @@
         <a:xfrm>
           <a:off x="4573576" y="2509984"/>
           <a:ext cx="10516746" cy="1685995"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>16061</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>174431</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>8775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A917997-53BC-48C5-9A76-F01FB95ADB81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3926914" y="3659460"/>
+          <a:ext cx="10548655" cy="1708158"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2221,8 +2296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434DFAFE-DE46-4ACE-9F95-A3B27799B338}">
   <dimension ref="B3:T18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2240,18 +2315,18 @@
   <sheetData>
     <row r="3" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="4" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="50">
+      <c r="D4" s="27">
         <v>512</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B5" s="51"/>
+      <c r="B5" s="29"/>
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
@@ -2260,27 +2335,27 @@
       </c>
     </row>
     <row r="6" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="49"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="28">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B7" s="48" t="s">
+      <c r="B7" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="50">
+      <c r="D7" s="27">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B8" s="51"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
@@ -2289,7 +2364,7 @@
       </c>
     </row>
     <row r="9" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B9" s="49"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="15" t="s">
         <v>22</v>
       </c>
@@ -2298,18 +2373,18 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="29" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="23">
         <v>4</v>
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="B11" s="51"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
@@ -2318,7 +2393,7 @@
       </c>
     </row>
     <row r="12" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="49"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="15" t="s">
         <v>22</v>
       </c>
@@ -2328,120 +2403,115 @@
     </row>
     <row r="14" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="15" spans="2:20" x14ac:dyDescent="0.35">
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="31" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="21" t="s">
+      <c r="I15" s="48"/>
+      <c r="J15" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="K15" s="21"/>
-      <c r="L15" s="20" t="s">
+      <c r="K15" s="50"/>
+      <c r="L15" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="M15" s="20"/>
+      <c r="M15" s="48"/>
       <c r="N15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="22" t="s">
+      <c r="O15" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="P15" s="23" t="s">
+      <c r="P15" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="Q15" s="24" t="s">
+      <c r="Q15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="R15" s="25" t="s">
+      <c r="R15" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="S15" s="25"/>
-      <c r="T15" s="26"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="43"/>
     </row>
     <row r="16" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F16" s="49"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="43"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="44"/>
-      <c r="P16" s="45"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="26"/>
       <c r="Q16" s="15"/>
-      <c r="R16" s="29" t="s">
+      <c r="R16" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="S16" s="46"/>
-      <c r="T16" s="47"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="45"/>
     </row>
     <row r="17" spans="6:20" x14ac:dyDescent="0.35">
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="H17" s="35"/>
-      <c r="I17" s="36" t="s">
+      <c r="H17" s="49"/>
+      <c r="I17" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="J17" s="36"/>
-      <c r="K17" s="35" t="s">
+      <c r="J17" s="40"/>
+      <c r="K17" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="36" t="s">
+      <c r="L17" s="49"/>
+      <c r="M17" s="49"/>
+      <c r="N17" s="49"/>
+      <c r="O17" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="P17" s="36"/>
-      <c r="Q17" s="37" t="s">
+      <c r="P17" s="40"/>
+      <c r="Q17" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="R17" s="37"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="38" t="s">
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="23" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="6:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="F18" s="49"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="29" t="s">
+      <c r="F18" s="30"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="34" t="s">
         <v>42</v>
       </c>
-      <c r="J18" s="30"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="29" t="s">
+      <c r="J18" s="35"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="33"/>
-      <c r="S18" s="34"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="39"/>
       <c r="T18" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
     <mergeCell ref="K18:N18"/>
     <mergeCell ref="O18:P18"/>
     <mergeCell ref="Q18:S18"/>
@@ -2458,6 +2528,11 @@
     <mergeCell ref="L15:M15"/>
     <mergeCell ref="K17:N17"/>
     <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="I18:J18"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="J16:K16"/>
   </mergeCells>

</xml_diff>